<commit_message>
Adding a more simple tab for testing purposes
</commit_message>
<xml_diff>
--- a/BookToValidate03.xlsx
+++ b/BookToValidate03.xlsx
@@ -5,19 +5,21 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/712e76bdfa434146/Documents/githubProjects/validator/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ChaibgalliCl_3jx4l8\OneDrive\Documents\githubProjects\validator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="125" documentId="13_ncr:1_{BEE77D52-8FC8-46A4-AB66-33C9950B804E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{84D883B0-AA2E-4B77-B866-80087A2A20A7}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B954FEC4-6BD9-41B5-AB94-188F7EC147D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{48B41AE7-338C-46D3-B278-C9ABE81569C3}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{48B41AE7-338C-46D3-B278-C9ABE81569C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Book_01" sheetId="1" r:id="rId1"/>
-    <sheet name="Dummy_Tab" sheetId="2" r:id="rId2"/>
+    <sheet name="Book_02" sheetId="3" r:id="rId2"/>
+    <sheet name="Dummy_Tab" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Book_01!$B$1:$B$34</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Book_02!$B$1:$B$2</definedName>
     <definedName name="Index">#REF!</definedName>
     <definedName name="Start_1">#REF!</definedName>
     <definedName name="Start_10">#REF!</definedName>
@@ -46,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="171">
   <si>
     <t>US/Canada</t>
   </si>
@@ -995,7 +997,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE5218D5-9F32-4A80-8491-65FEDECEA1DF}">
   <dimension ref="A1:E59"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2003,6 +2005,82 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9CE16F4-9A2C-49D2-8804-4F1D9DDB8607}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="5" width="25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection formatColumns="0" autoFilter="0"/>
+  <autoFilter ref="B1:B2" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
+  <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;P / &amp;N</oddFooter>
+    <evenFooter>&amp;C&amp;P / &amp;N</evenFooter>
+    <firstFooter>&amp;C&amp;P / &amp;N</firstFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E1393D1-B1EF-4E0F-8DAE-E4F45F5A6CAF}">
   <dimension ref="A1:D3"/>
   <sheetViews>

</xml_diff>